<commit_message>
added deterministic flag equals true to predict functions
</commit_message>
<xml_diff>
--- a/HyperParameter Tuned CartPole.xlsx
+++ b/HyperParameter Tuned CartPole.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chirag\Desktop\gitstuff\HyperTuned CartPole\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AEB659-43FA-4419-AF75-4C06FD701A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67967639-385E-4C14-9B72-E1FEF98767BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D1B170E5-861E-4102-9EA7-938F0BDED469}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D1B170E5-861E-4102-9EA7-938F0BDED469}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="CartPole" sheetId="1" r:id="rId1"/>
+    <sheet name="Trading" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Model Type</t>
   </si>
@@ -54,6 +56,15 @@
   </si>
   <si>
     <t>*3x Improvement</t>
+  </si>
+  <si>
+    <t>AnyTrading Return (Training Data Only)</t>
+  </si>
+  <si>
+    <t>No Hyperparameter Tuning PPO (1000 timesteps)</t>
+  </si>
+  <si>
+    <t>Hyperparameter Tuned PPO (1000 timesteps)</t>
   </si>
 </sst>
 </file>
@@ -173,7 +184,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$F$3</c:f>
+              <c:f>CartPole!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -251,7 +262,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$E$4:$E$7</c:f>
+              <c:f>CartPole!$E$4:$E$7</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -271,7 +282,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$F$4:$F$7</c:f>
+              <c:f>CartPole!$F$4:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -293,6 +304,352 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F3E8-4BDA-A2A5-EC3249F74A89}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="832564424"/>
+        <c:axId val="597822440"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="832564424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="597822440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="597822440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="832564424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Trading!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AnyTrading Return (Training Data Only)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Trading!$E$4:$E$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Hyperparameter Tuned PPO (30000 timesteps)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hyperparameter Tuned PPO (1000 timesteps)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>No Hyperparameter Tuning PPO (1000 timesteps)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Random Action Sample</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Trading!$F$4:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>73.59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>73.59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-64.59</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-96.59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3826-4BC6-B7B1-2439845402A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -503,7 +860,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1027,6 +1927,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{630456DC-C39B-4458-AC89-124DFFBDF6DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA493825-D2D1-4A47-A81C-EB5D4D319BA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1348,8 +2291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC84EFA6-8EAF-4CC0-83A1-7CA5EDFD2E71}">
   <dimension ref="E3:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1408,4 +2351,67 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA77C0F5-5CA0-4B89-A6DB-14A0F22CF3AB}">
+  <dimension ref="E3:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="42.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>73.59</v>
+      </c>
+    </row>
+    <row r="5" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>73.59</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>-64.59</v>
+      </c>
+    </row>
+    <row r="7" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>-96.59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>